<commit_message>
Updated Iteration 3 sprint backlog
I assigned myself tasks that I would like to work on and estimated the time to finish each.
</commit_message>
<xml_diff>
--- a/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
+++ b/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Documents\HealthCareSync\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jabes\Downloads\HealthCareSync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84227817-3949-420B-80D4-C580E4DB6422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662109AA-87E7-4534-9D7D-7CB85873BC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="1545" windowWidth="16380" windowHeight="18030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Related User Story</t>
   </si>
@@ -1723,20 +1723,20 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="18" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="15"/>
+    <col min="1" max="1" width="51.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.453125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="34.7265625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" style="18" customWidth="1"/>
+    <col min="6" max="9" width="9.1796875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -1759,7 +1759,7 @@
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
     </row>
-    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24"/>
       <c r="B2" s="23"/>
       <c r="C2" s="1" t="s">
@@ -1782,7 +1782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
@@ -1805,7 +1805,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
@@ -1815,14 +1815,18 @@
       <c r="C4" s="13">
         <v>1</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="D4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="13">
+        <v>14</v>
+      </c>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
@@ -1839,7 +1843,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -1849,14 +1853,18 @@
       <c r="C6" s="13">
         <v>2</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="D6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="13">
+        <v>4</v>
+      </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1866,14 +1874,18 @@
       <c r="C7" s="13">
         <v>3</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="D7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="13">
+        <v>4</v>
+      </c>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1892,7 +1904,7 @@
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -1911,7 +1923,7 @@
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1930,7 +1942,7 @@
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="5"/>
       <c r="C11" s="4"/>
@@ -1941,7 +1953,7 @@
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1951,7 +1963,7 @@
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" s="7"/>
       <c r="C13" s="14"/>
       <c r="D13" s="16"/>
@@ -1986,6 +1998,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041FBA4D6976FF34697CED57BA3121E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90eba6b134f98a2dcd6f2554d0702a0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7" xmlns:ns4="3bea4f68-df9b-425b-8be9-897e521449f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b10b116c70102c4d21148cc2133431f" ns3:_="" ns4:_="">
     <xsd:import namespace="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7"/>
@@ -2232,15 +2253,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2248,6 +2260,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61A29E-1F26-4720-A5C6-A54EFA5CA6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2262,14 +2282,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated my (ahmad's) time remaining hours
Updated my (ahmad's) time remaining hours
</commit_message>
<xml_diff>
--- a/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
+++ b/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jabes\Downloads\HealthCareSync\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Documents\HealthCareSync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662109AA-87E7-4534-9D7D-7CB85873BC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B383697B-D5CD-426A-83C9-7EE717B633DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2505" yWindow="1545" windowWidth="16380" windowHeight="18030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1722,21 +1722,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.453125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="34.7265625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" style="18" customWidth="1"/>
-    <col min="6" max="9" width="9.1796875" style="15"/>
+    <col min="1" max="1" width="51.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="18" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -1759,7 +1759,7 @@
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
     </row>
-    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" s="23"/>
       <c r="C2" s="1" t="s">
@@ -1782,7 +1782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
@@ -1801,11 +1801,13 @@
       <c r="F3" s="19">
         <v>7</v>
       </c>
-      <c r="G3" s="19"/>
+      <c r="G3" s="19">
+        <v>0</v>
+      </c>
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
@@ -1826,7 +1828,7 @@
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
@@ -1843,7 +1845,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -1864,7 +1866,7 @@
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1885,7 +1887,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1904,7 +1906,7 @@
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -1923,7 +1925,7 @@
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
     </row>
-    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1942,7 +1944,7 @@
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="5"/>
       <c r="C11" s="4"/>
@@ -1953,7 +1955,7 @@
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1963,7 +1965,7 @@
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
       <c r="C13" s="14"/>
       <c r="D13" s="16"/>
@@ -1998,15 +2000,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041FBA4D6976FF34697CED57BA3121E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90eba6b134f98a2dcd6f2554d0702a0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7" xmlns:ns4="3bea4f68-df9b-425b-8be9-897e521449f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b10b116c70102c4d21148cc2133431f" ns3:_="" ns4:_="">
     <xsd:import namespace="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7"/>
@@ -2253,6 +2246,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2260,14 +2262,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61A29E-1F26-4720-A5C6-A54EFA5CA6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2282,6 +2276,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Designed ManageAppts and update NursesHomePage UI
Converted ManageAppts from Form to UserControl, adding new UI elements and event handlers. enabled AutoScroll for mainPanel. Added LoadManageAppointments method and updated manageAppt_Click event handler.
</commit_message>
<xml_diff>
--- a/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
+++ b/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jabes\Downloads\HealthCareSync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662109AA-87E7-4534-9D7D-7CB85873BC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B6941C-A2EA-455C-8DB2-4773A861B3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1723,7 +1723,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1998,15 +1998,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041FBA4D6976FF34697CED57BA3121E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90eba6b134f98a2dcd6f2554d0702a0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7" xmlns:ns4="3bea4f68-df9b-425b-8be9-897e521449f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b10b116c70102c4d21148cc2133431f" ns3:_="" ns4:_="">
     <xsd:import namespace="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7"/>
@@ -2253,6 +2244,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2260,14 +2260,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61A29E-1F26-4720-A5C6-A54EFA5CA6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2282,6 +2274,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fixed bugs with AdminAddNurse
</commit_message>
<xml_diff>
--- a/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
+++ b/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jabes\Downloads\HealthCareSync\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Documents\HealthCareSync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B6941C-A2EA-455C-8DB2-4773A861B3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB62F8C9-582F-4FB3-BD3F-2A679F3D36D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="675" yWindow="2025" windowWidth="16380" windowHeight="18030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Related User Story</t>
   </si>
@@ -394,6 +394,9 @@
   </si>
   <si>
     <t>Jabesi</t>
+  </si>
+  <si>
+    <t>Rahman/Ahmad</t>
   </si>
 </sst>
 </file>
@@ -669,7 +672,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1723,20 +1726,20 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.453125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="34.7265625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" style="18" customWidth="1"/>
-    <col min="6" max="9" width="9.1796875" style="15"/>
+    <col min="1" max="1" width="51.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="18" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -1759,7 +1762,7 @@
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
     </row>
-    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" s="23"/>
       <c r="C2" s="1" t="s">
@@ -1782,7 +1785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
@@ -1805,7 +1808,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
@@ -1826,7 +1829,7 @@
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
@@ -1836,14 +1839,20 @@
       <c r="C5" s="13">
         <v>1</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="19"/>
+      <c r="D5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="13">
+        <v>14</v>
+      </c>
+      <c r="F5" s="19">
+        <v>14</v>
+      </c>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -1864,7 +1873,7 @@
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1885,7 +1894,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1904,7 +1913,7 @@
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -1915,15 +1924,21 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
+        <v>31</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="21">
+        <v>1</v>
+      </c>
+      <c r="G9" s="21">
+        <v>0</v>
+      </c>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
     </row>
-    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1942,7 +1957,7 @@
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="5"/>
       <c r="C11" s="4"/>
@@ -1953,7 +1968,7 @@
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1963,14 +1978,14 @@
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
       <c r="C13" s="14"/>
       <c r="D13" s="16"/>
       <c r="E13" s="17"/>
       <c r="F13" s="16">
         <f>SUM(F3:F12)</f>
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="G13" s="16">
         <f>SUM(G3:G12)</f>
@@ -1998,6 +2013,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041FBA4D6976FF34697CED57BA3121E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90eba6b134f98a2dcd6f2554d0702a0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7" xmlns:ns4="3bea4f68-df9b-425b-8be9-897e521449f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b10b116c70102c4d21148cc2133431f" ns3:_="" ns4:_="">
     <xsd:import namespace="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7"/>
@@ -2244,15 +2268,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2260,6 +2275,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61A29E-1F26-4720-A5C6-A54EFA5CA6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2274,14 +2297,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Refactor ViewModels and Update UI Layouts
Refactored `AppointmentViewModel.cs` to improve error messaging and streamline the appointment editing process.
Enhanced `LoginViewModel.cs` for better login handling and user feedback.
Updated `AdminHomePage.Designer.cs` and `AdminHomePage.cs` to adjust layout and remove redundant code.
Improved data binding and error handling in `ManageAppts.cs`. Enhanced layout and UI elements in `ManageNurses.Designer.cs` and other related files.
</commit_message>
<xml_diff>
--- a/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
+++ b/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Documents\HealthCareSync\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jabes\Downloads\HealthCareSync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01D4F6A-C1CC-49E2-BC9A-1F19D0273CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F62A5C-DF1F-49F8-9647-C9CAC0FE7367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="2025" windowWidth="16380" windowHeight="18030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Related User Story</t>
   </si>
@@ -397,6 +397,12 @@
   </si>
   <si>
     <t>Rahman/Ahmad</t>
+  </si>
+  <si>
+    <t>30'</t>
+  </si>
+  <si>
+    <t>10'</t>
   </si>
 </sst>
 </file>
@@ -672,13 +678,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1725,21 +1731,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="18" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="15"/>
+    <col min="1" max="1" width="51.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.453125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="34.7265625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" style="18" customWidth="1"/>
+    <col min="6" max="9" width="9.1796875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -1762,7 +1768,7 @@
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
     </row>
-    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24"/>
       <c r="B2" s="23"/>
       <c r="C2" s="1" t="s">
@@ -1785,7 +1791,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
@@ -1808,7 +1814,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
@@ -1824,12 +1830,18 @@
       <c r="E4" s="13">
         <v>14</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="F4" s="19">
+        <v>5</v>
+      </c>
+      <c r="G4" s="19">
+        <v>6</v>
+      </c>
+      <c r="H4" s="19">
+        <v>4</v>
+      </c>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
@@ -1852,7 +1864,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -1868,12 +1880,18 @@
       <c r="E6" s="13">
         <v>4</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
+      <c r="F6" s="19">
+        <v>0</v>
+      </c>
+      <c r="G6" s="19">
+        <v>3</v>
+      </c>
+      <c r="H6" s="19">
+        <v>1</v>
+      </c>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1889,12 +1907,18 @@
       <c r="E7" s="13">
         <v>4</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
+      <c r="F7" s="19">
+        <v>0</v>
+      </c>
+      <c r="G7" s="19">
+        <v>4</v>
+      </c>
+      <c r="H7" s="19">
+        <v>2</v>
+      </c>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1907,13 +1931,21 @@
       <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="21">
+        <v>0</v>
+      </c>
+      <c r="G8" s="21">
+        <v>0</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="I8" s="21"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -1938,7 +1970,7 @@
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1957,7 +1989,7 @@
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="5"/>
       <c r="C11" s="4"/>
@@ -1968,7 +2000,7 @@
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1978,22 +2010,22 @@
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" s="7"/>
       <c r="C13" s="14"/>
       <c r="D13" s="16"/>
       <c r="E13" s="17"/>
       <c r="F13" s="16">
         <f>SUM(F3:F12)</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G13" s="16">
         <f>SUM(G3:G12)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H13" s="16">
         <f>SUM(H3:H12)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I13" s="16">
         <f>SUM(I3:I12)</f>
@@ -2013,6 +2045,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041FBA4D6976FF34697CED57BA3121E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90eba6b134f98a2dcd6f2554d0702a0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7" xmlns:ns4="3bea4f68-df9b-425b-8be9-897e521449f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b10b116c70102c4d21148cc2133431f" ns3:_="" ns4:_="">
     <xsd:import namespace="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7"/>
@@ -2259,15 +2300,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2275,6 +2307,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61A29E-1F26-4720-A5C6-A54EFA5CA6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2289,14 +2329,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated sprint backlog to iteration 4 and added nurse_id to routine checks table
Updated sprint backlog to iteration 4 and added nurse_id to routine checks table and modified code to update having nurse_id in the routine checks table
</commit_message>
<xml_diff>
--- a/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
+++ b/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Ahmad\HealthCareSync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0009D379-F064-4997-A177-30607CB2EDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3924D3-B1D9-4AAD-A28D-42CC82446BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="2025" windowWidth="16380" windowHeight="18030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Related User Story</t>
   </si>
@@ -59,19 +59,16 @@
     <t>Amount Remaining After…</t>
   </si>
   <si>
-    <t>Assignee</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
     <t>Level</t>
   </si>
   <si>
-    <t>Create an appointment</t>
-  </si>
-  <si>
-    <t>Enter routine checkup information</t>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>Enter initial diagnosis and order tests for a visit</t>
   </si>
   <si>
     <r>
@@ -93,7 +90,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Design Routine Checks UI </t>
+      <t xml:space="preserve"> Before the user confirms the tests ordered, the user can remove or add more tests to the order. Note that initial diagnosis is optional at the routine checkup stage. The nurse can fill in it later after the doctor exams the patient. </t>
     </r>
     <r>
       <rPr>
@@ -104,6 +101,189 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Design UI </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Add functionality to enter intial diagnosis and order tests</t>
+    </r>
+  </si>
+  <si>
+    <t>Enter Test results</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Design UI </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Add functionality to be able to enter test results</t>
+    </r>
+  </si>
+  <si>
+    <t>Enter final diagnosis</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Once the final diagnosis is entered, patient visit information such as the checkup, tests, and diagnosis is read-only. Make sure to prompt the user about it for confirmation. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Design UI </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Add functionality to be able to enter final diagnosis</t>
+    </r>
+  </si>
+  <si>
+    <t>Search patients and view patients' visit information</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Search patients and view patients' visit information (e.g checkup info., tests ordered and/or performed including time, diagnoses, etc. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">2. </t>
     </r>
     <r>
@@ -114,16 +294,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Add functionality to enter routine checks information and store it in the database (keep in mind systolic, diastolic blood pressure and pulse are integer values, weight (lb), height (in) is a decimal value)</t>
-    </r>
-  </si>
-  <si>
-    <t>Search for patient to show his/her appointment information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search for a patient by criteria </t>
-  </si>
-  <si>
+      <t xml:space="preserve">Design UI </t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -133,18 +305,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Add Search UI elements into the Manage_Patients form </t>
-    </r>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Add functionality to search and view patients' visit information</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -154,6 +328,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> admin edit nurse (including updating nurse's password), delete nurse (if there is no visit associated with the nurse, otherwise, deactivate the nurse) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>2.</t>
     </r>
     <r>
@@ -164,10 +359,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Add functionality to search by date of birth, name (last and first), or both (note that the search should be done on the DB server side instead of the client side )</t>
-    </r>
-  </si>
-  <si>
+      <t xml:space="preserve"> Design UI </t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -177,232 +370,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Design Search UI. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Add functionality to search for patients and display their appointment information (same search criteria as above)</t>
-    </r>
-  </si>
-  <si>
-    <t>Edit Appointment if time has not passed</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Design edit appointment UI. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Add functionality to edit an appointment only if the time hasn't passed and save those changes to the database</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Design create appointment UI </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Add functionality to create appointments and save them in the database(Double booking isn't allowed and appointments are 20 minutes long)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Ahmad </t>
-  </si>
-  <si>
-    <t>Initial</t>
-  </si>
-  <si>
-    <t>Estimate</t>
-  </si>
-  <si>
-    <t>Display username</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Display username in the UI </t>
-    </r>
-  </si>
-  <si>
-    <t>Fix Add Nurse</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Fix the bugs with adding a nurse</t>
-    </r>
-  </si>
-  <si>
-    <t>Fix Nurse state text box</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nurse state box should be a comboBox/dropdownBox instead of text box</t>
-    </r>
-  </si>
-  <si>
-    <t>Rahman</t>
-  </si>
-  <si>
-    <t>Jabesi</t>
-  </si>
-  <si>
-    <t>Rahman/Ahmad</t>
-  </si>
-  <si>
-    <t>30'</t>
-  </si>
-  <si>
-    <t>10'</t>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Add functionality to edit nurse and delete/deactivate nurse</t>
+    </r>
+  </si>
+  <si>
+    <t>Admin edit/delete/deactivate nurse</t>
+  </si>
+  <si>
+    <t>Assignees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial </t>
+  </si>
+  <si>
+    <t>ITERATION 4 DESCRIPTION NOTES:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">note that please be concious about the user-friendlines of your program. It's not user-friendly if the user only sees ids without any detailed information.  It's important that on all the views, it should be clear about
+    the patient's name, dob
+    doctor's name
+    nurse's name
+Each team member must use at least one stored procedure for one of the DB operations for this iteration so that everyone may practice writing stored procedures and see how it helps you reduce the coupling of the SQL statement that would otherwise have been embedded in your code. Please have the stored procedures in the readme.txt file for easy access during the demo. </t>
   </si>
 </sst>
 </file>
@@ -482,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -555,6 +553,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,13 +679,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1729,10 +1730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,10 +1754,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>21</v>
@@ -1772,11 +1773,11 @@
       <c r="A2" s="24"/>
       <c r="B2" s="23"/>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F2" s="20" t="s">
         <v>2</v>
@@ -1791,202 +1792,116 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" s="13">
-        <v>2</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="13">
-        <v>7</v>
-      </c>
-      <c r="F3" s="19">
-        <v>7</v>
-      </c>
-      <c r="G3" s="19">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C4" s="13">
         <v>1</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="13">
-        <v>14</v>
-      </c>
-      <c r="F4" s="19">
-        <v>5</v>
-      </c>
-      <c r="G4" s="19">
-        <v>6</v>
-      </c>
-      <c r="H4" s="19">
-        <v>4</v>
-      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="19"/>
     </row>
     <row r="5" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" s="13">
         <v>1</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="13">
-        <v>14</v>
-      </c>
-      <c r="F5" s="19">
-        <v>14</v>
-      </c>
-      <c r="G5" s="19">
-        <v>0</v>
-      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="13">
         <v>2</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="13">
-        <v>4</v>
-      </c>
-      <c r="F6" s="19">
-        <v>0</v>
-      </c>
-      <c r="G6" s="19">
-        <v>3</v>
-      </c>
-      <c r="H6" s="19">
-        <v>1</v>
-      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="13">
-        <v>3</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="13">
-        <v>4</v>
-      </c>
-      <c r="F7" s="19">
-        <v>0</v>
-      </c>
-      <c r="G7" s="19">
-        <v>4</v>
-      </c>
-      <c r="H7" s="19">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
       <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="4">
-        <v>4</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="21">
-        <v>0</v>
-      </c>
-      <c r="G8" s="21">
-        <v>0</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>33</v>
-      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="4">
-        <v>4</v>
-      </c>
-      <c r="F9" s="21">
-        <v>4</v>
-      </c>
-      <c r="G9" s="21">
-        <v>0</v>
-      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="4">
-        <v>3</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>29</v>
-      </c>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
@@ -2021,19 +1936,29 @@
       <c r="E13" s="17"/>
       <c r="F13" s="16">
         <f>SUM(F3:F12)</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G13" s="16">
         <f>SUM(G3:G12)</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="H13" s="16">
         <f>SUM(H3:H12)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I13" s="16">
         <f>SUM(I3:I12)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="270" x14ac:dyDescent="0.25">
+      <c r="B15" s="25" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2049,6 +1974,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041FBA4D6976FF34697CED57BA3121E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90eba6b134f98a2dcd6f2554d0702a0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7" xmlns:ns4="3bea4f68-df9b-425b-8be9-897e521449f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b10b116c70102c4d21148cc2133431f" ns3:_="" ns4:_="">
     <xsd:import namespace="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7"/>
@@ -2295,15 +2229,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2311,6 +2236,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61A29E-1F26-4720-A5C6-A54EFA5CA6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2325,14 +2258,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Assign myself with "Enter test result" task.
</commit_message>
<xml_diff>
--- a/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
+++ b/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Ahmad\HealthCareSync\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr00096\source\repos\HealthCareSync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3924D3-B1D9-4AAD-A28D-42CC82446BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB051CC-973E-47AE-9C3C-C3A716995E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="9885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Related User Story</t>
   </si>
@@ -401,6 +401,9 @@
     doctor's name
     nurse's name
 Each team member must use at least one stored procedure for one of the DB operations for this iteration so that everyone may practice writing stored procedures and see how it helps you reduce the coupling of the SQL statement that would otherwise have been embedded in your code. Please have the stored procedures in the readme.txt file for easy access during the demo. </t>
+  </si>
+  <si>
+    <t>Md Mostafizur Rahman</t>
   </si>
 </sst>
 </file>
@@ -545,6 +548,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -553,9 +559,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1733,7 +1736,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1747,10 +1750,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1762,16 +1765,16 @@
       <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="24"/>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1819,8 +1822,12 @@
       <c r="C4" s="13">
         <v>1</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="D4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="13">
+        <v>5</v>
+      </c>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
@@ -1957,7 +1964,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="270" x14ac:dyDescent="0.25">
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="22" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1974,15 +1981,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041FBA4D6976FF34697CED57BA3121E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90eba6b134f98a2dcd6f2554d0702a0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7" xmlns:ns4="3bea4f68-df9b-425b-8be9-897e521449f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b10b116c70102c4d21148cc2133431f" ns3:_="" ns4:_="">
     <xsd:import namespace="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7"/>
@@ -2229,6 +2227,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2236,14 +2243,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61A29E-1F26-4720-A5C6-A54EFA5CA6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2258,6 +2257,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Modifing the lab_test table and add permanent value too it.
</commit_message>
<xml_diff>
--- a/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
+++ b/Documents/Health Care Sys Sprint 1 (Iteration 3)  Backlog Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr00096\source\repos\HealthCareSync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB051CC-973E-47AE-9C3C-C3A716995E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045C8D92-EC58-400B-847A-CC261A6CB76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="9885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Related User Story</t>
   </si>
@@ -404,6 +404,12 @@
   </si>
   <si>
     <t>Md Mostafizur Rahman</t>
+  </si>
+  <si>
+    <t>Modifing the lab_test table and add permanent value too it.</t>
+  </si>
+  <si>
+    <t>Redesign the database.</t>
   </si>
 </sst>
 </file>
@@ -682,7 +688,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1735,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1885,11 +1891,24 @@
       <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="21"/>
+      <c r="A8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2</v>
+      </c>
+      <c r="F8" s="21">
+        <v>1</v>
+      </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
@@ -1943,7 +1962,7 @@
       <c r="E13" s="17"/>
       <c r="F13" s="16">
         <f>SUM(F3:F12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="16">
         <f>SUM(G3:G12)</f>
@@ -1981,6 +2000,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041FBA4D6976FF34697CED57BA3121E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90eba6b134f98a2dcd6f2554d0702a0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7" xmlns:ns4="3bea4f68-df9b-425b-8be9-897e521449f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b10b116c70102c4d21148cc2133431f" ns3:_="" ns4:_="">
     <xsd:import namespace="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7"/>
@@ -2227,15 +2255,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2243,6 +2262,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61A29E-1F26-4720-A5C6-A54EFA5CA6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2257,14 +2284,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>